<commit_message>
aggiornamento csv e xlsx dstaspxn
</commit_message>
<xml_diff>
--- a/DSTASPXN.xlsx
+++ b/DSTASPXN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gruppofsitaliane-my.sharepoint.com/personal/8931520_fstechnology_it/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_B171291DA95470AEC90A337243C63ED420F8EB9D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD8C661D-6A4F-4598-A0B2-AC151D094A77}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_B1717125EE6D342FC83E6B9353C63ED420F8DF08" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1827F41C-AAA1-4590-927C-74E57BCC57F1}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9446" uniqueCount="9439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9450" uniqueCount="9443">
   <si>
     <t>dsvccr</t>
   </si>
@@ -28337,6 +28337,18 @@
   </si>
   <si>
     <t>SAN DANIELE DEL FRIULI</t>
+  </si>
+  <si>
+    <t>14701</t>
+  </si>
+  <si>
+    <t>PESCARA AEROPORTO</t>
+  </si>
+  <si>
+    <t>14600</t>
+  </si>
+  <si>
+    <t>GRADARA</t>
   </si>
 </sst>
 </file>
@@ -28685,7 +28697,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4723"/>
+  <dimension ref="A1:B4725"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:AN1048576"/>
@@ -28693,8 +28705,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="41.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -66481,6 +66493,22 @@
         <v>9438</v>
       </c>
     </row>
+    <row r="4724" spans="1:2">
+      <c r="A4724" t="s">
+        <v>9439</v>
+      </c>
+      <c r="B4724" t="s">
+        <v>9440</v>
+      </c>
+    </row>
+    <row r="4725" spans="1:2">
+      <c r="A4725" t="s">
+        <v>9441</v>
+      </c>
+      <c r="B4725" t="s">
+        <v>9442</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
aggiornamenti al codice, ora il salvataggio del csv finale è sul desktop ed è stata aggiornata la lista delle localitò su dstaspxn
</commit_message>
<xml_diff>
--- a/DSTASPXN.xlsx
+++ b/DSTASPXN.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gruppofsitaliane-my.sharepoint.com/personal/8931520_fstechnology_it/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gruppofsitaliane-my.sharepoint.com/personal/8931520_fstechnology_it/Documents/Documenti/csv_editor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_B1717125EE6D342FC83E6B9353C63ED420F8DF08" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1827F41C-AAA1-4590-927C-74E57BCC57F1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4A1D82FE-32A1-410F-B385-4152A9A3454E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9450" uniqueCount="9443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9460" uniqueCount="9453">
   <si>
     <t>dsvccr</t>
   </si>
@@ -28234,109 +28234,109 @@
     <t>14601</t>
   </si>
   <si>
-    <t>UDINE AUTOSTAZIONE</t>
+    <t>UDINE AUTOSTAZIONE (BUS)</t>
   </si>
   <si>
     <t>14602</t>
   </si>
   <si>
-    <t>CASANOVA DI MARTIGNACCO</t>
+    <t>CASANOVA DI MARTIGNACCO (BUS)</t>
   </si>
   <si>
     <t>14603</t>
   </si>
   <si>
-    <t>PLAINO</t>
+    <t>PLAINO (BUS)</t>
   </si>
   <si>
     <t>14604</t>
   </si>
   <si>
-    <t>TORREANO DI MARTIGNACCO</t>
+    <t>TORREANO DI MARTIGNACCO (BUS)</t>
   </si>
   <si>
     <t>14605</t>
   </si>
   <si>
-    <t>CERESETTO</t>
+    <t>CERESETTO (BUS)</t>
   </si>
   <si>
     <t>14606</t>
   </si>
   <si>
-    <t>MARTIGNACCO</t>
+    <t>MARTIGNACCO (BUS)</t>
   </si>
   <si>
     <t>14607</t>
   </si>
   <si>
-    <t>VILLALTA DI FAGAGNA</t>
+    <t>VILLALTA DI FAGAGNA (BUS)</t>
   </si>
   <si>
     <t>14608</t>
   </si>
   <si>
-    <t>CICONICCO</t>
+    <t>CICONICCO (BUS)</t>
   </si>
   <si>
     <t>14609</t>
   </si>
   <si>
-    <t>FAGAGNA</t>
+    <t>FAGAGNA (BUS)</t>
   </si>
   <si>
     <t>14610</t>
   </si>
   <si>
-    <t>SAN GIOVANNI IN COLLE</t>
+    <t>SAN GIOVANNI IN COLLE (BUS)</t>
   </si>
   <si>
     <t>14611</t>
   </si>
   <si>
-    <t>BATTAGLIA DI FAGAGNA</t>
+    <t>BATTAGLIA DI FAGAGNA (BUS)</t>
   </si>
   <si>
     <t>14612</t>
   </si>
   <si>
-    <t>MADRISIO DI FAGAGNA</t>
+    <t>MADRISIO DI FAGAGNA (BUS)</t>
   </si>
   <si>
     <t>14613</t>
   </si>
   <si>
-    <t>POZZALIS</t>
+    <t>POZZALIS (BUS)</t>
   </si>
   <si>
     <t>14614</t>
   </si>
   <si>
-    <t>RIVE D'ARCANO</t>
+    <t>RIVE D'ARCANO (BUS)</t>
   </si>
   <si>
     <t>14615</t>
   </si>
   <si>
-    <t>RIVOTTA</t>
+    <t>RIVOTTA (BUS)</t>
   </si>
   <si>
     <t>14616</t>
   </si>
   <si>
-    <t>RODEANO BASSO</t>
+    <t>RODEANO BASSO (BUS)</t>
   </si>
   <si>
     <t>14617</t>
   </si>
   <si>
-    <t>RODEANO ALTO</t>
+    <t>RODEANO ALTO (BUS)</t>
   </si>
   <si>
     <t>14618</t>
   </si>
   <si>
-    <t>SAN DANIELE DEL FRIULI</t>
+    <t>SAN DANIELE DEL FRIULI (BUS)</t>
   </si>
   <si>
     <t>14701</t>
@@ -28349,6 +28349,36 @@
   </si>
   <si>
     <t>GRADARA</t>
+  </si>
+  <si>
+    <t>14599</t>
+  </si>
+  <si>
+    <t>CORTONA CENTRO - PIAZZA MERCATO</t>
+  </si>
+  <si>
+    <t>14598</t>
+  </si>
+  <si>
+    <t>CORTONA CENTRO - PIAZZA GARIBALDI</t>
+  </si>
+  <si>
+    <t>14702</t>
+  </si>
+  <si>
+    <t>TRTEC07-CORTONA</t>
+  </si>
+  <si>
+    <t>14703</t>
+  </si>
+  <si>
+    <t>VALMONTONE OUTLET</t>
+  </si>
+  <si>
+    <t>14704</t>
+  </si>
+  <si>
+    <t>AGRIGENTO SCUOLE</t>
   </si>
 </sst>
 </file>
@@ -28697,17 +28727,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4725"/>
+  <dimension ref="A1:B4730"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:AN1048576"/>
+      <selection activeCell="C1" sqref="C1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="41.28515625" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -66509,6 +66535,46 @@
         <v>9442</v>
       </c>
     </row>
+    <row r="4726" spans="1:2">
+      <c r="A4726" t="s">
+        <v>9443</v>
+      </c>
+      <c r="B4726" t="s">
+        <v>9444</v>
+      </c>
+    </row>
+    <row r="4727" spans="1:2">
+      <c r="A4727" t="s">
+        <v>9445</v>
+      </c>
+      <c r="B4727" t="s">
+        <v>9446</v>
+      </c>
+    </row>
+    <row r="4728" spans="1:2">
+      <c r="A4728" t="s">
+        <v>9447</v>
+      </c>
+      <c r="B4728" t="s">
+        <v>9448</v>
+      </c>
+    </row>
+    <row r="4729" spans="1:2">
+      <c r="A4729" t="s">
+        <v>9449</v>
+      </c>
+      <c r="B4729" t="s">
+        <v>9450</v>
+      </c>
+    </row>
+    <row r="4730" spans="1:2">
+      <c r="A4730" t="s">
+        <v>9451</v>
+      </c>
+      <c r="B4730" t="s">
+        <v>9452</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>